<commit_message>
VH-00 - Ajustes do Back-end
</commit_message>
<xml_diff>
--- a/documentos/documento-de-layout/Documento de layout.xlsx
+++ b/documentos/documento-de-layout/Documento de layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laris\Desktop\PROJETO-3ºS\BandTec-3ADSA-2021-2-Grupo-05\documentos\documento-de-layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE722E3-8C89-492D-B11A-72D58BA64526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEC2EA8-BD01-4CB9-931A-71ED85C4A6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{4BAB5A63-40E4-46BD-BD60-CAA7630584D5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="100">
   <si>
     <t xml:space="preserve">Nº. do campo </t>
   </si>
@@ -301,12 +301,6 @@
     <t>003-032</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>033-050</t>
-  </si>
-  <si>
     <t>033-039</t>
   </si>
   <si>
@@ -320,6 +314,27 @@
   </si>
   <si>
     <t>103-357</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>043-057</t>
+  </si>
+  <si>
+    <t>058-072</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>033-046</t>
+  </si>
+  <si>
+    <t>073-157</t>
+  </si>
+  <si>
+    <t>85</t>
   </si>
 </sst>
 </file>
@@ -769,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BCECD9-81BD-43DD-BBEE-7E67D5DA14B1}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E568E1-FCC9-4397-ADD4-B116B908D12D}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F40" sqref="A33:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,10 +1268,10 @@
         <v>74</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>9</v>
@@ -1424,7 +1439,7 @@
         <v>50</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>34</v>
@@ -1444,7 +1459,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>20</v>
@@ -1464,7 +1479,7 @@
         <v>60</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>9</v>
@@ -1484,7 +1499,7 @@
         <v>60</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>9</v>
@@ -1504,7 +1519,7 @@
         <v>68</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>9</v>
@@ -1607,6 +1622,166 @@
       </c>
       <c r="D30" s="4" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>3</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP: Integracao certified seller + Integracao-validacoes tela profile seller + implementacao exportacao e importacao arquivo txt + implementacao fila + ajustes gerais css + 'limpeza' no codigo
</commit_message>
<xml_diff>
--- a/documentos/documento-de-layout/Documento de layout.xlsx
+++ b/documentos/documento-de-layout/Documento de layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laris\Desktop\PROJETO-3ºS\BandTec-3ADSA-2021-2-Grupo-05\documentos\documento-de-layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEC2EA8-BD01-4CB9-931A-71ED85C4A6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59238476-A5AE-483E-BD27-BD4AF5FBE489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{4BAB5A63-40E4-46BD-BD60-CAA7630584D5}"/>
+    <workbookView xWindow="4170" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{4BAB5A63-40E4-46BD-BD60-CAA7630584D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Exportação" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
VH-00 - Ajustes gerais na app + correcao de BUGS
</commit_message>
<xml_diff>
--- a/documentos/documento-de-layout/Documento de layout.xlsx
+++ b/documentos/documento-de-layout/Documento de layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laris\Desktop\PROJETO-3ºS\BandTec-3ADSA-2021-2-Grupo-05\documentos\documento-de-layout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laris\Desktop\PROJETO-4ºS\BandTec-3ADSA-2021-2-Grupo-05\documentos\documento-de-layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59238476-A5AE-483E-BD27-BD4AF5FBE489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18242A08-6CDC-426A-A192-FC5D2017483D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{4BAB5A63-40E4-46BD-BD60-CAA7630584D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4BAB5A63-40E4-46BD-BD60-CAA7630584D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Exportação" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="101">
   <si>
     <t xml:space="preserve">Nº. do campo </t>
   </si>
@@ -331,10 +331,13 @@
     <t>033-046</t>
   </si>
   <si>
-    <t>073-157</t>
-  </si>
-  <si>
     <t>85</t>
+  </si>
+  <si>
+    <t>058-142</t>
+  </si>
+  <si>
+    <t>78-332</t>
   </si>
 </sst>
 </file>
@@ -782,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BCECD9-81BD-43DD-BBEE-7E67D5DA14B1}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,59 +1125,60 @@
         <v>42</v>
       </c>
       <c r="B19" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C22" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="20" t="s">
+      <c r="E22" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1185,10 +1189,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E568E1-FCC9-4397-ADD4-B116B908D12D}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F40" sqref="A33:F40"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,39 +1753,39 @@
         <v>41</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D41" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="5" t="s">
+      <c r="E41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>